<commit_message>
Water quality lab added data.
</commit_message>
<xml_diff>
--- a/groundwater/data-raw/waterquality/2017/STRIPS2017groundwaterresults.xlsx
+++ b/groundwater/data-raw/waterquality/2017/STRIPS2017groundwaterresults.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\my.files.iastate.edu\cals\NREM\Buffer\Share\Students\Leigh Ann Long\WQRL\STRIPS\STRIPS 2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\prairiestrips\groundwater\data-raw\waterquality\2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171026"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Long, Leigh A [ABE]</author>
+    <author>Leigh Long</author>
   </authors>
   <commentList>
     <comment ref="A51" authorId="0" shapeId="0">
@@ -77,12 +78,43 @@
         </r>
       </text>
     </comment>
+    <comment ref="E185" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Refilter and reanalyze sample.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A210" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Missing sample.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>STRIPs 2017 groundwater analysis results</t>
+  </si>
   <si>
     <t>Sample ID#</t>
   </si>
@@ -93,19 +125,16 @@
     <t>NOx result (mg N/L)</t>
   </si>
   <si>
-    <t>STRIPs 2017 groundwater analysis results</t>
+    <t>Dissolved reactive phosphorus analysis date</t>
   </si>
   <si>
     <t>DRP result (mg P/L)</t>
-  </si>
-  <si>
-    <t>Dissolved reactive phosphorus analysis date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -215,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -234,21 +263,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="84">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="83">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1355,10 +1375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E168"/>
+  <dimension ref="A1:E213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="G107" sqref="G107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C196" sqref="C196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,24 +1392,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3857,7 +3877,12 @@
       <c r="A150">
         <v>6145</v>
       </c>
-      <c r="C150" s="1"/>
+      <c r="B150" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C150" s="1">
+        <v>10.894500000000001</v>
+      </c>
       <c r="D150" s="3">
         <v>43010</v>
       </c>
@@ -3869,7 +3894,12 @@
       <c r="A151">
         <v>6146</v>
       </c>
-      <c r="C151" s="1"/>
+      <c r="B151" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C151" s="1">
+        <v>6.9546000000000001</v>
+      </c>
       <c r="D151" s="3">
         <v>43010</v>
       </c>
@@ -3881,7 +3911,12 @@
       <c r="A152">
         <v>6147</v>
       </c>
-      <c r="C152" s="1"/>
+      <c r="B152" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C152" s="1">
+        <v>4.5571000000000002</v>
+      </c>
       <c r="D152" s="3">
         <v>43010</v>
       </c>
@@ -3893,7 +3928,12 @@
       <c r="A153">
         <v>6148</v>
       </c>
-      <c r="C153" s="1"/>
+      <c r="B153" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C153" s="1">
+        <v>5.4915000000000003</v>
+      </c>
       <c r="D153" s="3">
         <v>43010</v>
       </c>
@@ -3905,7 +3945,12 @@
       <c r="A154">
         <v>6149</v>
       </c>
-      <c r="C154" s="1"/>
+      <c r="B154" s="3">
+        <v>43109</v>
+      </c>
+      <c r="C154" s="12">
+        <v>0.16200000000000001</v>
+      </c>
       <c r="D154" s="3">
         <v>43010</v>
       </c>
@@ -3917,7 +3962,12 @@
       <c r="A155">
         <v>6150</v>
       </c>
-      <c r="C155" s="1"/>
+      <c r="B155" s="3">
+        <v>43109</v>
+      </c>
+      <c r="C155" s="12">
+        <v>2.8000000000000001E-2</v>
+      </c>
       <c r="D155" s="3">
         <v>43010</v>
       </c>
@@ -3929,7 +3979,12 @@
       <c r="A156">
         <v>6151</v>
       </c>
-      <c r="C156" s="1"/>
+      <c r="B156" s="3">
+        <v>43109</v>
+      </c>
+      <c r="C156" s="12">
+        <v>0.124</v>
+      </c>
       <c r="D156" s="3">
         <v>43010</v>
       </c>
@@ -3941,7 +3996,12 @@
       <c r="A157">
         <v>6152</v>
       </c>
-      <c r="C157" s="1"/>
+      <c r="B157" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C157" s="12">
+        <v>6.0768000000000004</v>
+      </c>
       <c r="D157" s="3">
         <v>43010</v>
       </c>
@@ -3953,7 +4013,12 @@
       <c r="A158">
         <v>6153</v>
       </c>
-      <c r="C158" s="1"/>
+      <c r="B158" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C158" s="12">
+        <v>9.0433000000000003</v>
+      </c>
       <c r="D158" s="3">
         <v>43010</v>
       </c>
@@ -3965,7 +4030,12 @@
       <c r="A159">
         <v>6154</v>
       </c>
-      <c r="C159" s="1"/>
+      <c r="B159" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C159" s="12">
+        <v>1.7040999999999999</v>
+      </c>
       <c r="D159" s="3">
         <v>43010</v>
       </c>
@@ -3977,7 +4047,12 @@
       <c r="A160">
         <v>6155</v>
       </c>
-      <c r="C160" s="1"/>
+      <c r="B160" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C160" s="12">
+        <v>13.1875</v>
+      </c>
       <c r="D160" s="3">
         <v>43010</v>
       </c>
@@ -3989,7 +4064,12 @@
       <c r="A161">
         <v>6156</v>
       </c>
-      <c r="C161" s="1"/>
+      <c r="B161" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C161" s="12">
+        <v>1.4883</v>
+      </c>
       <c r="D161" s="3">
         <v>43010</v>
       </c>
@@ -4001,7 +4081,12 @@
       <c r="A162">
         <v>6157</v>
       </c>
-      <c r="C162" s="1"/>
+      <c r="B162" s="3">
+        <v>43109</v>
+      </c>
+      <c r="C162" s="12">
+        <v>0.26700000000000002</v>
+      </c>
       <c r="D162" s="3">
         <v>43010</v>
       </c>
@@ -4013,7 +4098,12 @@
       <c r="A163">
         <v>6158</v>
       </c>
-      <c r="C163" s="1"/>
+      <c r="B163" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C163" s="12">
+        <v>0.35620000000000002</v>
+      </c>
       <c r="D163" s="3">
         <v>43010</v>
       </c>
@@ -4025,7 +4115,12 @@
       <c r="A164">
         <v>6159</v>
       </c>
-      <c r="C164" s="1"/>
+      <c r="B164" s="3">
+        <v>43109</v>
+      </c>
+      <c r="C164" s="12">
+        <v>6.8000000000000005E-2</v>
+      </c>
       <c r="D164" s="3">
         <v>43010</v>
       </c>
@@ -4037,7 +4132,12 @@
       <c r="A165">
         <v>6160</v>
       </c>
-      <c r="C165" s="1"/>
+      <c r="B165" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C165" s="12">
+        <v>9.5356000000000005</v>
+      </c>
       <c r="D165" s="3">
         <v>43010</v>
       </c>
@@ -4049,7 +4149,12 @@
       <c r="A166">
         <v>6161</v>
       </c>
-      <c r="C166" s="1"/>
+      <c r="B166" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C166" s="12">
+        <v>8.3657000000000004</v>
+      </c>
       <c r="D166" s="3">
         <v>43010</v>
       </c>
@@ -4061,7 +4166,12 @@
       <c r="A167">
         <v>6162</v>
       </c>
-      <c r="C167" s="1"/>
+      <c r="B167" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C167" s="12">
+        <v>11.9506</v>
+      </c>
       <c r="D167" s="3">
         <v>43010</v>
       </c>
@@ -4073,7 +4183,12 @@
       <c r="A168">
         <v>6163</v>
       </c>
-      <c r="C168" s="1"/>
+      <c r="B168" s="3">
+        <v>43052</v>
+      </c>
+      <c r="C168" s="12">
+        <v>13.0732</v>
+      </c>
       <c r="D168" s="3">
         <v>43010</v>
       </c>
@@ -4081,419 +4196,1071 @@
         <v>5.5E-2</v>
       </c>
     </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>6164</v>
+      </c>
+      <c r="B169" s="3">
+        <v>43109</v>
+      </c>
+      <c r="C169" s="12">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="D169" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E169" s="1">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>6165</v>
+      </c>
+      <c r="B170" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C170" s="12">
+        <v>0.27229999999999999</v>
+      </c>
+      <c r="D170" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E170" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>6166</v>
+      </c>
+      <c r="B171" s="3">
+        <v>43109</v>
+      </c>
+      <c r="C171" s="12">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="D171" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E171" s="1">
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>6167</v>
+      </c>
+      <c r="B172" s="3">
+        <v>43109</v>
+      </c>
+      <c r="C172" s="12">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="D172" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E172" s="1">
+        <v>0.29399999999999998</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>6168</v>
+      </c>
+      <c r="B173" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C173" s="12">
+        <v>6.8234000000000004</v>
+      </c>
+      <c r="D173" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E173" s="1">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>6169</v>
+      </c>
+      <c r="B174" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C174" s="12">
+        <v>3.6882999999999999</v>
+      </c>
+      <c r="D174" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E174" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>6170</v>
+      </c>
+      <c r="B175" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C175" s="12">
+        <v>4.1174999999999997</v>
+      </c>
+      <c r="D175" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E175" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>6171</v>
+      </c>
+      <c r="B176" s="3">
+        <v>43109</v>
+      </c>
+      <c r="C176" s="12">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D176" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E176" s="1">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>6172</v>
+      </c>
+      <c r="B177" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C177" s="12">
+        <v>5.2069000000000001</v>
+      </c>
+      <c r="D177" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E177" s="1">
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>6173</v>
+      </c>
+      <c r="B178" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C178" s="12">
+        <v>4.2897999999999996</v>
+      </c>
+      <c r="D178" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E178" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>6174</v>
+      </c>
+      <c r="B179" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C179" s="12">
+        <v>2.5529999999999999</v>
+      </c>
+      <c r="D179" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E179" s="1">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>6175</v>
+      </c>
+      <c r="B180" s="3">
+        <v>43109</v>
+      </c>
+      <c r="C180" s="12">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D180" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E180" s="1">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>6176</v>
+      </c>
+      <c r="B181" s="3">
+        <v>43109</v>
+      </c>
+      <c r="C181" s="12">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="D181" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E181" s="1">
+        <v>0.45500000000000002</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>6177</v>
+      </c>
+      <c r="B182" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C182" s="12">
+        <v>4.7805</v>
+      </c>
+      <c r="D182" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E182" s="1">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>6178</v>
+      </c>
+      <c r="B183" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C183" s="12">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="D183" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E183" s="1">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>6179</v>
+      </c>
+      <c r="B184" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C184" s="12">
+        <v>2.7517999999999998</v>
+      </c>
+      <c r="D184" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E184" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>6180</v>
+      </c>
+      <c r="B185" s="3">
+        <v>43109</v>
+      </c>
+      <c r="C185" s="12">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="D185" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E185" s="8">
+        <v>1.2669999999999999</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>6181</v>
+      </c>
+      <c r="B186" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C186" s="1">
+        <v>5.7667000000000002</v>
+      </c>
+      <c r="D186" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E186" s="1">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>6182</v>
+      </c>
+      <c r="B187" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C187" s="1">
+        <v>5.2603</v>
+      </c>
+      <c r="D187" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E187" s="1">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>6183</v>
+      </c>
+      <c r="B188" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C188" s="1">
+        <v>1.5608</v>
+      </c>
+      <c r="D188" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E188" s="1">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>6184</v>
+      </c>
+      <c r="B189" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C189" s="1">
+        <v>1.1040000000000001</v>
+      </c>
+      <c r="D189" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E189" s="1">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>6185</v>
+      </c>
+      <c r="B190" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C190" s="1">
+        <v>11.7753</v>
+      </c>
+      <c r="D190" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E190" s="1">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>6186</v>
+      </c>
+      <c r="B191" s="3">
+        <v>43049</v>
+      </c>
+      <c r="C191" s="1">
+        <v>8.0213000000000001</v>
+      </c>
+      <c r="D191" s="3">
+        <v>43055</v>
+      </c>
+      <c r="E191" s="1">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>6187</v>
+      </c>
+      <c r="B192" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C192" s="1">
+        <v>9.8079999999999998</v>
+      </c>
+      <c r="E192" s="1"/>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>6188</v>
+      </c>
+      <c r="B193" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C193" s="1">
+        <v>7.319</v>
+      </c>
+      <c r="E193" s="1"/>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>6189</v>
+      </c>
+      <c r="B194" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C194" s="1">
+        <v>3.7189999999999999</v>
+      </c>
+      <c r="E194" s="1"/>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>6190</v>
+      </c>
+      <c r="B195" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C195" s="1">
+        <v>4.9930000000000003</v>
+      </c>
+      <c r="E195" s="1"/>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>6191</v>
+      </c>
+      <c r="B196" s="3">
+        <v>43109</v>
+      </c>
+      <c r="C196" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="E196" s="1"/>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>6192</v>
+      </c>
+      <c r="B197" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C197" s="1">
+        <v>1.161</v>
+      </c>
+      <c r="E197" s="1"/>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>6193</v>
+      </c>
+      <c r="B198" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C198" s="1">
+        <v>0.378</v>
+      </c>
+      <c r="E198" s="1"/>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>6194</v>
+      </c>
+      <c r="B199" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C199" s="1">
+        <v>6.5170000000000003</v>
+      </c>
+      <c r="E199" s="1"/>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>6195</v>
+      </c>
+      <c r="B200" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C200" s="1">
+        <v>8.6110000000000007</v>
+      </c>
+      <c r="E200" s="1"/>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>6196</v>
+      </c>
+      <c r="B201" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C201" s="1">
+        <v>1.089</v>
+      </c>
+      <c r="E201" s="1"/>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>6197</v>
+      </c>
+      <c r="B202" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C202" s="1">
+        <v>13.647</v>
+      </c>
+      <c r="E202" s="1"/>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>6198</v>
+      </c>
+      <c r="B203" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C203" s="1">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="E203" s="1"/>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>6199</v>
+      </c>
+      <c r="B204" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C204" s="1">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="E204" s="1"/>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>6200</v>
+      </c>
+      <c r="B205" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C205" s="1">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="E205" s="1"/>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>6201</v>
+      </c>
+      <c r="B206" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C206" s="1">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="E206" s="1"/>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>6202</v>
+      </c>
+      <c r="B207" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C207" s="1">
+        <v>10.113</v>
+      </c>
+      <c r="E207" s="1"/>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>6203</v>
+      </c>
+      <c r="B208" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C208" s="1">
+        <v>8.766</v>
+      </c>
+      <c r="E208" s="1"/>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>6204</v>
+      </c>
+      <c r="B209" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C209" s="1">
+        <v>13.558</v>
+      </c>
+      <c r="E209" s="1"/>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="7">
+        <v>6205</v>
+      </c>
+      <c r="B210" s="7"/>
+      <c r="C210" s="8"/>
+      <c r="D210" s="7"/>
+      <c r="E210" s="8"/>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>6206</v>
+      </c>
+      <c r="B211" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C211" s="1">
+        <v>12.443</v>
+      </c>
+      <c r="E211" s="1"/>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>6207</v>
+      </c>
+      <c r="B212" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C212" s="1">
+        <v>4.95</v>
+      </c>
+      <c r="E212" s="1"/>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>6208</v>
+      </c>
+      <c r="B213" s="3">
+        <v>43108</v>
+      </c>
+      <c r="C213" s="1">
+        <v>7.6260000000000003</v>
+      </c>
+      <c r="E213" s="1"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C11 C31:C33 C35:C39">
-    <cfRule type="cellIs" dxfId="83" priority="84" operator="lessThan">
+    <cfRule type="cellIs" dxfId="82" priority="84" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="82" priority="83" operator="lessThan">
+    <cfRule type="cellIs" dxfId="81" priority="83" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:C20">
-    <cfRule type="cellIs" dxfId="81" priority="82" operator="lessThan">
+    <cfRule type="cellIs" dxfId="80" priority="82" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="80" priority="81" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="81" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C29">
-    <cfRule type="cellIs" dxfId="79" priority="80" operator="lessThan">
+    <cfRule type="cellIs" dxfId="78" priority="80" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="cellIs" dxfId="78" priority="79" operator="lessThan">
+    <cfRule type="cellIs" dxfId="77" priority="79" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="77" priority="77" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="77" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="76" priority="76" operator="lessThan">
+    <cfRule type="cellIs" dxfId="75" priority="76" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:C44 C47:C49">
-    <cfRule type="cellIs" dxfId="75" priority="75" operator="lessThan">
+    <cfRule type="cellIs" dxfId="74" priority="75" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="cellIs" dxfId="74" priority="74" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="74" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:C58">
-    <cfRule type="cellIs" dxfId="73" priority="73" operator="lessThan">
+    <cfRule type="cellIs" dxfId="72" priority="73" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="72" priority="72" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="72" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C63">
-    <cfRule type="cellIs" dxfId="71" priority="71" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="71" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66:C73">
-    <cfRule type="cellIs" dxfId="70" priority="70" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="70" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="cellIs" dxfId="69" priority="69" operator="lessThan">
+    <cfRule type="cellIs" dxfId="68" priority="69" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75:C82">
-    <cfRule type="cellIs" dxfId="68" priority="68" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="68" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83">
-    <cfRule type="cellIs" dxfId="67" priority="67" operator="lessThan">
+    <cfRule type="cellIs" dxfId="66" priority="67" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C84 C87:C91">
-    <cfRule type="cellIs" dxfId="66" priority="66" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="66" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92">
-    <cfRule type="cellIs" dxfId="65" priority="65" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="65" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C93 C95:C100">
-    <cfRule type="cellIs" dxfId="64" priority="64" operator="lessThan">
+    <cfRule type="cellIs" dxfId="63" priority="64" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="cellIs" dxfId="63" priority="63" operator="lessThan">
+    <cfRule type="cellIs" dxfId="62" priority="63" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C102">
-    <cfRule type="cellIs" dxfId="62" priority="62" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="62" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="61" priority="61" operator="lessThan">
+    <cfRule type="cellIs" dxfId="60" priority="61" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:C65">
-    <cfRule type="cellIs" dxfId="60" priority="60" operator="lessThan">
+    <cfRule type="cellIs" dxfId="59" priority="60" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C85:C86">
-    <cfRule type="cellIs" dxfId="59" priority="59" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="59" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94">
-    <cfRule type="cellIs" dxfId="58" priority="58" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="58" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E126:E133">
-    <cfRule type="cellIs" dxfId="57" priority="57" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="57" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="cellIs" dxfId="56" priority="56" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="56" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E135:E142">
-    <cfRule type="cellIs" dxfId="55" priority="55" operator="lessThan">
+    <cfRule type="cellIs" dxfId="54" priority="55" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E143">
-    <cfRule type="cellIs" dxfId="54" priority="54" operator="lessThan">
+    <cfRule type="cellIs" dxfId="53" priority="54" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144:E149">
-    <cfRule type="cellIs" dxfId="53" priority="53" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="53" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E99:E106">
-    <cfRule type="cellIs" dxfId="52" priority="52" operator="lessThan">
+    <cfRule type="cellIs" dxfId="51" priority="52" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E108">
-    <cfRule type="cellIs" dxfId="51" priority="51" operator="lessThan">
+    <cfRule type="cellIs" dxfId="50" priority="51" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109:E116">
-    <cfRule type="cellIs" dxfId="50" priority="50" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E117">
-    <cfRule type="cellIs" dxfId="49" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="49" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E125">
-    <cfRule type="cellIs" dxfId="48" priority="48" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="48" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52:E59">
-    <cfRule type="cellIs" dxfId="47" priority="47" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="cellIs" dxfId="46" priority="46" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="46" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61:E68">
-    <cfRule type="cellIs" dxfId="45" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69">
-    <cfRule type="cellIs" dxfId="44" priority="44" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70:E77">
-    <cfRule type="cellIs" dxfId="43" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="43" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78">
-    <cfRule type="cellIs" dxfId="42" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="42" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E79:E86">
-    <cfRule type="cellIs" dxfId="41" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="cellIs" dxfId="40" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88:E95">
-    <cfRule type="cellIs" dxfId="39" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E96">
-    <cfRule type="cellIs" dxfId="38" priority="38" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="38" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97:E98">
-    <cfRule type="cellIs" dxfId="37" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="37" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E11">
-    <cfRule type="cellIs" dxfId="36" priority="36" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="35" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13:E20">
-    <cfRule type="cellIs" dxfId="34" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="34" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="33" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:E29">
-    <cfRule type="cellIs" dxfId="32" priority="32" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="31" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="31" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:E33">
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:E39">
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41:E47">
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="27" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C125:C132">
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C133">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C137:C141">
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C142">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C143 C145:C149">
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103:C105">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C108 C110:C111">
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C112">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C114:C117 C119:C120">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C121">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C122:C124">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C109">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C113">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C118">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C134:C136">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C144">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E150:E157">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E158">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E159:E166">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E167">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E168">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Created graphs for Guthrie
</commit_message>
<xml_diff>
--- a/groundwater/data-raw/waterquality/2017/STRIPS2017groundwaterresults.xlsx
+++ b/groundwater/data-raw/waterquality/2017/STRIPS2017groundwaterresults.xlsx
@@ -88,11 +88,57 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>Refilter and reanalyze sample.</t>
+          <t xml:space="preserve">Sediment present in filtered sample; refilter and reanalyze sample -&gt; done as of 1/18/18.
+</t>
         </r>
       </text>
     </comment>
     <comment ref="A210" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Missing sample.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C218" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Will reanalyze 1/23/18.
+Done as of 1/25/18.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E268" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Sediment present in filtered sample; refilter and reanalyze sample -&gt; done as of 1/19/18.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A294" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -175,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -240,11 +286,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -264,11 +330,65 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="83">
+  <dxfs count="88">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1375,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E213"/>
+  <dimension ref="A1:E296"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C196" sqref="C196"/>
+    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
+      <selection activeCell="B234" sqref="B234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4362,7 +4482,7 @@
       <c r="D178" s="3">
         <v>43055</v>
       </c>
-      <c r="E178" s="1">
+      <c r="E178" s="6">
         <v>0.01</v>
       </c>
     </row>
@@ -4379,7 +4499,7 @@
       <c r="D179" s="3">
         <v>43055</v>
       </c>
-      <c r="E179" s="1">
+      <c r="E179" s="6">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
@@ -4396,7 +4516,7 @@
       <c r="D180" s="3">
         <v>43055</v>
       </c>
-      <c r="E180" s="1">
+      <c r="E180" s="6">
         <v>1.6E-2</v>
       </c>
     </row>
@@ -4413,7 +4533,7 @@
       <c r="D181" s="3">
         <v>43055</v>
       </c>
-      <c r="E181" s="1">
+      <c r="E181" s="6">
         <v>0.45500000000000002</v>
       </c>
     </row>
@@ -4430,7 +4550,7 @@
       <c r="D182" s="3">
         <v>43055</v>
       </c>
-      <c r="E182" s="1">
+      <c r="E182" s="6">
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
@@ -4447,7 +4567,7 @@
       <c r="D183" s="3">
         <v>43055</v>
       </c>
-      <c r="E183" s="1">
+      <c r="E183" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
@@ -4464,7 +4584,7 @@
       <c r="D184" s="3">
         <v>43055</v>
       </c>
-      <c r="E184" s="1">
+      <c r="E184" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
@@ -4479,10 +4599,10 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="D185" s="3">
-        <v>43055</v>
-      </c>
-      <c r="E185" s="8">
-        <v>1.2669999999999999</v>
+        <v>43118</v>
+      </c>
+      <c r="E185" s="6">
+        <v>0.66200000000000003</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -4498,7 +4618,7 @@
       <c r="D186" s="3">
         <v>43055</v>
       </c>
-      <c r="E186" s="1">
+      <c r="E186" s="6">
         <v>0.03</v>
       </c>
     </row>
@@ -4597,7 +4717,12 @@
       <c r="C192" s="1">
         <v>9.8079999999999998</v>
       </c>
-      <c r="E192" s="1"/>
+      <c r="D192" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E192" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193">
@@ -4609,7 +4734,12 @@
       <c r="C193" s="1">
         <v>7.319</v>
       </c>
-      <c r="E193" s="1"/>
+      <c r="D193" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E193" s="1">
+        <v>2E-3</v>
+      </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194">
@@ -4621,7 +4751,12 @@
       <c r="C194" s="1">
         <v>3.7189999999999999</v>
       </c>
-      <c r="E194" s="1"/>
+      <c r="D194" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E194" s="1">
+        <v>1E-3</v>
+      </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195">
@@ -4633,7 +4768,12 @@
       <c r="C195" s="1">
         <v>4.9930000000000003</v>
       </c>
-      <c r="E195" s="1"/>
+      <c r="D195" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E195" s="1">
+        <v>2E-3</v>
+      </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196">
@@ -4645,7 +4785,12 @@
       <c r="C196" s="12">
         <v>0.14499999999999999</v>
       </c>
-      <c r="E196" s="1"/>
+      <c r="D196" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E196" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197">
@@ -4657,7 +4802,12 @@
       <c r="C197" s="1">
         <v>1.161</v>
       </c>
-      <c r="E197" s="1"/>
+      <c r="D197" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E197" s="1">
+        <v>1.6E-2</v>
+      </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198">
@@ -4669,7 +4819,12 @@
       <c r="C198" s="1">
         <v>0.378</v>
       </c>
-      <c r="E198" s="1"/>
+      <c r="D198" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E198" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199">
@@ -4681,7 +4836,12 @@
       <c r="C199" s="1">
         <v>6.5170000000000003</v>
       </c>
-      <c r="E199" s="1"/>
+      <c r="D199" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E199" s="1">
+        <v>3.9E-2</v>
+      </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200">
@@ -4693,7 +4853,12 @@
       <c r="C200" s="1">
         <v>8.6110000000000007</v>
       </c>
-      <c r="E200" s="1"/>
+      <c r="D200" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E200" s="1">
+        <v>3.2000000000000001E-2</v>
+      </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201">
@@ -4705,7 +4870,12 @@
       <c r="C201" s="1">
         <v>1.089</v>
       </c>
-      <c r="E201" s="1"/>
+      <c r="D201" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E201" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202">
@@ -4717,7 +4887,12 @@
       <c r="C202" s="1">
         <v>13.647</v>
       </c>
-      <c r="E202" s="1"/>
+      <c r="D202" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E202" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203">
@@ -4729,7 +4904,12 @@
       <c r="C203" s="1">
         <v>0.88300000000000001</v>
       </c>
-      <c r="E203" s="1"/>
+      <c r="D203" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E203" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204">
@@ -4741,7 +4921,12 @@
       <c r="C204" s="1">
         <v>0.83899999999999997</v>
       </c>
-      <c r="E204" s="1"/>
+      <c r="D204" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E204" s="1">
+        <v>8.9999999999999993E-3</v>
+      </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205">
@@ -4753,7 +4938,12 @@
       <c r="C205" s="1">
         <v>0.61699999999999999</v>
       </c>
-      <c r="E205" s="1"/>
+      <c r="D205" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E205" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206">
@@ -4765,7 +4955,12 @@
       <c r="C206" s="1">
         <v>0.39900000000000002</v>
       </c>
-      <c r="E206" s="1"/>
+      <c r="D206" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E206" s="1">
+        <v>1E-3</v>
+      </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207">
@@ -4777,7 +4972,12 @@
       <c r="C207" s="1">
         <v>10.113</v>
       </c>
-      <c r="E207" s="1"/>
+      <c r="D207" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E207" s="1">
+        <v>1.7999999999999999E-2</v>
+      </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208">
@@ -4789,7 +4989,12 @@
       <c r="C208" s="1">
         <v>8.766</v>
       </c>
-      <c r="E208" s="1"/>
+      <c r="D208" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E208" s="1">
+        <v>0.14899999999999999</v>
+      </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209">
@@ -4801,7 +5006,12 @@
       <c r="C209" s="1">
         <v>13.558</v>
       </c>
-      <c r="E209" s="1"/>
+      <c r="D209" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E209" s="1">
+        <v>2.5999999999999999E-2</v>
+      </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="7">
@@ -4822,7 +5032,12 @@
       <c r="C211" s="1">
         <v>12.443</v>
       </c>
-      <c r="E211" s="1"/>
+      <c r="D211" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E211" s="6">
+        <v>5.0999999999999997E-2</v>
+      </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212">
@@ -4831,10 +5046,15 @@
       <c r="B212" s="3">
         <v>43108</v>
       </c>
-      <c r="C212" s="1">
+      <c r="C212" s="6">
         <v>4.95</v>
       </c>
-      <c r="E212" s="1"/>
+      <c r="D212" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E212" s="6">
+        <v>2.4E-2</v>
+      </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213">
@@ -4846,422 +5066,1855 @@
       <c r="C213" s="1">
         <v>7.6260000000000003</v>
       </c>
-      <c r="E213" s="1"/>
+      <c r="D213" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E213" s="6">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>6209</v>
+      </c>
+      <c r="B214" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C214" s="6">
+        <v>9.5329999999999995</v>
+      </c>
+      <c r="D214" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E214" s="6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>6210</v>
+      </c>
+      <c r="B215" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C215" s="6">
+        <v>6.7220000000000004</v>
+      </c>
+      <c r="D215" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E215" s="6">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>6211</v>
+      </c>
+      <c r="B216" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C216" s="6">
+        <v>3.2629999999999999</v>
+      </c>
+      <c r="D216" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E216" s="6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>6212</v>
+      </c>
+      <c r="B217" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C217" s="6">
+        <v>4.7789999999999999</v>
+      </c>
+      <c r="D217" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E217" s="6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>6213</v>
+      </c>
+      <c r="B218" s="3">
+        <v>43125</v>
+      </c>
+      <c r="C218" s="6">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="D218" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E218" s="6">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>6214</v>
+      </c>
+      <c r="B219" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C219" s="6">
+        <v>0.26</v>
+      </c>
+      <c r="D219" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E219" s="6">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>6215</v>
+      </c>
+      <c r="B220" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C220" s="6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D220" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E220" s="6">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>6216</v>
+      </c>
+      <c r="B221" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C221" s="6">
+        <v>2.3490000000000002</v>
+      </c>
+      <c r="D221" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E221" s="6">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>6217</v>
+      </c>
+      <c r="B222" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C222" s="6">
+        <v>9.1630000000000003</v>
+      </c>
+      <c r="D222" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E222" s="6">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>6218</v>
+      </c>
+      <c r="B223" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C223" s="6">
+        <v>0.47</v>
+      </c>
+      <c r="D223" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E223" s="6">
+        <v>8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>6219</v>
+      </c>
+      <c r="B224" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C224" s="6">
+        <v>21.15</v>
+      </c>
+      <c r="D224" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E224" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>6220</v>
+      </c>
+      <c r="B225" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C225" s="6">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="D225" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E225" s="6">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>6221</v>
+      </c>
+      <c r="B226" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C226" s="6">
+        <v>1.099</v>
+      </c>
+      <c r="D226" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E226" s="6">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>6222</v>
+      </c>
+      <c r="B227" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C227" s="6">
+        <v>1.401</v>
+      </c>
+      <c r="D227" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E227" s="6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>6223</v>
+      </c>
+      <c r="B228" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C228" s="6">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="D228" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E228" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>6224</v>
+      </c>
+      <c r="B229" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C229" s="6">
+        <v>9.6020000000000003</v>
+      </c>
+      <c r="D229" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E229" s="6">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>6225</v>
+      </c>
+      <c r="B230" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C230" s="6">
+        <v>6.1970000000000001</v>
+      </c>
+      <c r="D230" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E230" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>6226</v>
+      </c>
+      <c r="B231" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C231" s="6">
+        <v>11.189</v>
+      </c>
+      <c r="D231" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E231" s="6">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>6227</v>
+      </c>
+      <c r="B232" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C232" s="6">
+        <v>14.173</v>
+      </c>
+      <c r="D232" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E232" s="6">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>6228</v>
+      </c>
+      <c r="B233" s="3">
+        <v>43117</v>
+      </c>
+      <c r="C233" s="6">
+        <v>7.9260000000000002</v>
+      </c>
+      <c r="D233" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E233" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>6229</v>
+      </c>
+      <c r="B234" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C234" s="1">
+        <v>6.2050000000000001</v>
+      </c>
+      <c r="D234" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E234" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>6230</v>
+      </c>
+      <c r="B235" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C235" s="1">
+        <v>2.8359999999999999</v>
+      </c>
+      <c r="D235" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E235" s="6">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>6231</v>
+      </c>
+      <c r="B236" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C236" s="1">
+        <v>4.8410000000000002</v>
+      </c>
+      <c r="D236" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E236" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>6232</v>
+      </c>
+      <c r="B237" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C237" s="1">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="D237" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E237" s="6">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>6233</v>
+      </c>
+      <c r="B238" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C238" s="1">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="D238" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E238" s="6">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>6234</v>
+      </c>
+      <c r="B239" s="3">
+        <v>43125</v>
+      </c>
+      <c r="C239" s="1">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="D239" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E239" s="6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>6235</v>
+      </c>
+      <c r="B240" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C240" s="1">
+        <v>2.4079999999999999</v>
+      </c>
+      <c r="D240" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E240" s="6">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>6236</v>
+      </c>
+      <c r="B241" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C241" s="1">
+        <v>9.1769999999999996</v>
+      </c>
+      <c r="D241" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E241" s="6">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>6237</v>
+      </c>
+      <c r="B242" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C242" s="1">
+        <v>1.331</v>
+      </c>
+      <c r="D242" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E242" s="6">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>6238</v>
+      </c>
+      <c r="B243" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C243" s="1">
+        <v>15.848000000000001</v>
+      </c>
+      <c r="D243" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E243" s="6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>6239</v>
+      </c>
+      <c r="B244" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C244" s="1">
+        <v>0.253</v>
+      </c>
+      <c r="D244" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E244" s="6">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>6240</v>
+      </c>
+      <c r="B245" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C245" s="1">
+        <v>5.6449999999999996</v>
+      </c>
+      <c r="D245" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E245" s="6">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>6241</v>
+      </c>
+      <c r="B246" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C246" s="1">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="D246" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E246" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>6242</v>
+      </c>
+      <c r="B247" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C247" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="D247" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E247" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>6243</v>
+      </c>
+      <c r="B248" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C248" s="1">
+        <v>10.000999999999999</v>
+      </c>
+      <c r="D248" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E248" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>6244</v>
+      </c>
+      <c r="B249" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C249" s="1">
+        <v>4.5620000000000003</v>
+      </c>
+      <c r="D249" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E249" s="6">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>6245</v>
+      </c>
+      <c r="B250" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C250" s="1">
+        <v>10.872999999999999</v>
+      </c>
+      <c r="D250" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E250" s="6">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>6246</v>
+      </c>
+      <c r="B251" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C251" s="1">
+        <v>10.605</v>
+      </c>
+      <c r="D251" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E251" s="6">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>6247</v>
+      </c>
+      <c r="B252" s="3">
+        <v>43125</v>
+      </c>
+      <c r="C252" s="1">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="D252" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E252" s="6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>6248</v>
+      </c>
+      <c r="B253" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C253" s="1">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="D253" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E253" s="6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>6249</v>
+      </c>
+      <c r="B254" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C254" s="1">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="D254" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E254" s="6">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>6250</v>
+      </c>
+      <c r="B255" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C255" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="D255" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E255" s="6">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>6251</v>
+      </c>
+      <c r="B256" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C256" s="1">
+        <v>7.077</v>
+      </c>
+      <c r="D256" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E256" s="6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>6252</v>
+      </c>
+      <c r="B257" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C257" s="1">
+        <v>3.8740000000000001</v>
+      </c>
+      <c r="D257" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E257" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>6253</v>
+      </c>
+      <c r="B258" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C258" s="1">
+        <v>3.6629999999999998</v>
+      </c>
+      <c r="D258" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E258" s="6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>6254</v>
+      </c>
+      <c r="B259" s="3">
+        <v>43125</v>
+      </c>
+      <c r="C259" s="1">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="D259" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E259" s="6">
+        <v>0.223</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>6255</v>
+      </c>
+      <c r="B260" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C260" s="1">
+        <v>4.944</v>
+      </c>
+      <c r="D260" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E260" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>6256</v>
+      </c>
+      <c r="B261" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C261" s="1">
+        <v>4.2169999999999996</v>
+      </c>
+      <c r="D261" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E261" s="6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>6257</v>
+      </c>
+      <c r="B262" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C262" s="1">
+        <v>2.726</v>
+      </c>
+      <c r="D262" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E262" s="6">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>6258</v>
+      </c>
+      <c r="B263" s="3">
+        <v>43125</v>
+      </c>
+      <c r="C263" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="D263" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E263" s="6">
+        <v>0.23200000000000001</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>6259</v>
+      </c>
+      <c r="B264" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C264" s="1">
+        <v>2.4670000000000001</v>
+      </c>
+      <c r="D264" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E264" s="6">
+        <v>0.122</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>6260</v>
+      </c>
+      <c r="B265" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C265" s="1">
+        <v>5.1890000000000001</v>
+      </c>
+      <c r="D265" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E265" s="6">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>6261</v>
+      </c>
+      <c r="B266" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C266" s="1">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="D266" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E266" s="6">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>6262</v>
+      </c>
+      <c r="B267" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C267" s="1">
+        <v>4.8879999999999999</v>
+      </c>
+      <c r="D267" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E267" s="6">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>6263</v>
+      </c>
+      <c r="B268" s="3">
+        <v>43125</v>
+      </c>
+      <c r="C268" s="1">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="D268" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E268" s="6">
+        <v>1.095</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>6264</v>
+      </c>
+      <c r="B269" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C269" s="1">
+        <v>4.7290000000000001</v>
+      </c>
+      <c r="D269" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E269" s="6">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>6265</v>
+      </c>
+      <c r="B270" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C270" s="1">
+        <v>7.69</v>
+      </c>
+      <c r="D270" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E270" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>6266</v>
+      </c>
+      <c r="B271" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C271" s="1">
+        <v>6.2169999999999996</v>
+      </c>
+      <c r="D271" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E271" s="6">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>6267</v>
+      </c>
+      <c r="B272" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C272" s="1">
+        <v>1.746</v>
+      </c>
+      <c r="D272" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E272" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>6268</v>
+      </c>
+      <c r="B273" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C273" s="1">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="D273" s="3">
+        <v>43118</v>
+      </c>
+      <c r="E273" s="6">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>6269</v>
+      </c>
+      <c r="B274" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C274" s="1">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="D274" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E274" s="6">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>6270</v>
+      </c>
+      <c r="B275" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C275" s="1">
+        <v>8.0120000000000005</v>
+      </c>
+      <c r="D275" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E275" s="6">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>6271</v>
+      </c>
+      <c r="B276" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C276" s="1">
+        <v>8.9359999999999999</v>
+      </c>
+      <c r="D276" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E276" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>6272</v>
+      </c>
+      <c r="B277" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C277" s="1">
+        <v>6.3380000000000001</v>
+      </c>
+      <c r="D277" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E277" s="6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>6273</v>
+      </c>
+      <c r="B278" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C278" s="1">
+        <v>2.718</v>
+      </c>
+      <c r="D278" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E278" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>6274</v>
+      </c>
+      <c r="B279" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C279" s="1">
+        <v>4.53</v>
+      </c>
+      <c r="D279" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E279" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>6275</v>
+      </c>
+      <c r="B280" s="3">
+        <v>43125</v>
+      </c>
+      <c r="C280" s="1">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="D280" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E280" s="6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>6276</v>
+      </c>
+      <c r="B281" s="3">
+        <v>43125</v>
+      </c>
+      <c r="C281" s="1">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="D281" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E281" s="6">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>6277</v>
+      </c>
+      <c r="B282" s="3">
+        <v>43125</v>
+      </c>
+      <c r="C282" s="1">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="D282" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E282" s="6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>6278</v>
+      </c>
+      <c r="B283" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C283" s="1">
+        <v>1.615</v>
+      </c>
+      <c r="D283" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E283" s="6">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>6279</v>
+      </c>
+      <c r="B284" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C284" s="1">
+        <v>9.2579999999999991</v>
+      </c>
+      <c r="D284" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E284" s="6">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>6280</v>
+      </c>
+      <c r="B285" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C285" s="1">
+        <v>1.591</v>
+      </c>
+      <c r="D285" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E285" s="6">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>6281</v>
+      </c>
+      <c r="B286" s="3">
+        <v>43123</v>
+      </c>
+      <c r="C286" s="1">
+        <v>14.398999999999999</v>
+      </c>
+      <c r="D286" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E286" s="6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>6282</v>
+      </c>
+      <c r="B287" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C287" s="1">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="D287" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E287" s="6">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>6283</v>
+      </c>
+      <c r="B288" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C288" s="1">
+        <v>5.5549999999999997</v>
+      </c>
+      <c r="D288" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E288" s="6">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>6284</v>
+      </c>
+      <c r="B289" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C289" s="1">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="D289" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E289" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>6285</v>
+      </c>
+      <c r="B290" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C290" s="1">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="D290" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E290" s="6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>6286</v>
+      </c>
+      <c r="B291" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C291" s="1">
+        <v>9.9770000000000003</v>
+      </c>
+      <c r="D291" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E291" s="6">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>6287</v>
+      </c>
+      <c r="B292" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C292" s="1">
+        <v>4.2220000000000004</v>
+      </c>
+      <c r="D292" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E292" s="6">
+        <v>0.16700000000000001</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>6288</v>
+      </c>
+      <c r="B293" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C293" s="1">
+        <v>11.696999999999999</v>
+      </c>
+      <c r="D293" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E293" s="6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A294" s="7">
+        <v>6289</v>
+      </c>
+      <c r="B294" s="7"/>
+      <c r="C294" s="8"/>
+      <c r="D294" s="7"/>
+      <c r="E294" s="8"/>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>6290</v>
+      </c>
+      <c r="B295" s="3">
+        <v>43122</v>
+      </c>
+      <c r="C295" s="1">
+        <v>4.0679999999999996</v>
+      </c>
+      <c r="D295" s="3">
+        <v>43119</v>
+      </c>
+      <c r="E295" s="6">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A296" s="13">
+        <v>6291</v>
+      </c>
+      <c r="B296" s="15">
+        <v>43122</v>
+      </c>
+      <c r="C296" s="14">
+        <v>7.9669999999999996</v>
+      </c>
+      <c r="D296" s="15">
+        <v>43119</v>
+      </c>
+      <c r="E296" s="16">
+        <v>1.2999999999999999E-2</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C11 C31:C33 C35:C39">
-    <cfRule type="cellIs" dxfId="82" priority="84" operator="lessThan">
+    <cfRule type="cellIs" dxfId="87" priority="90" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
+    <cfRule type="cellIs" dxfId="86" priority="89" operator="lessThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:C20">
+    <cfRule type="cellIs" dxfId="85" priority="88" operator="lessThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="cellIs" dxfId="84" priority="87" operator="lessThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C29">
+    <cfRule type="cellIs" dxfId="83" priority="86" operator="lessThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="cellIs" dxfId="82" priority="85" operator="lessThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
     <cfRule type="cellIs" dxfId="81" priority="83" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:C20">
+  <conditionalFormatting sqref="C41">
     <cfRule type="cellIs" dxfId="80" priority="82" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
+  <conditionalFormatting sqref="C42:C44 C47:C49">
     <cfRule type="cellIs" dxfId="79" priority="81" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22:C29">
+  <conditionalFormatting sqref="C50">
     <cfRule type="cellIs" dxfId="78" priority="80" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
+  <conditionalFormatting sqref="C51:C58">
     <cfRule type="cellIs" dxfId="77" priority="79" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="76" priority="77" operator="lessThan">
+  <conditionalFormatting sqref="C59">
+    <cfRule type="cellIs" dxfId="76" priority="78" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="75" priority="76" operator="lessThan">
+  <conditionalFormatting sqref="C60:C63">
+    <cfRule type="cellIs" dxfId="75" priority="77" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42:C44 C47:C49">
-    <cfRule type="cellIs" dxfId="74" priority="75" operator="lessThan">
+  <conditionalFormatting sqref="C66:C73">
+    <cfRule type="cellIs" dxfId="74" priority="76" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="cellIs" dxfId="73" priority="74" operator="lessThan">
+  <conditionalFormatting sqref="C74">
+    <cfRule type="cellIs" dxfId="73" priority="75" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C51:C58">
-    <cfRule type="cellIs" dxfId="72" priority="73" operator="lessThan">
+  <conditionalFormatting sqref="C75:C82">
+    <cfRule type="cellIs" dxfId="72" priority="74" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="71" priority="72" operator="lessThan">
+  <conditionalFormatting sqref="C83">
+    <cfRule type="cellIs" dxfId="71" priority="73" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60:C63">
-    <cfRule type="cellIs" dxfId="70" priority="71" operator="lessThan">
+  <conditionalFormatting sqref="C84 C87:C91">
+    <cfRule type="cellIs" dxfId="70" priority="72" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C66:C73">
-    <cfRule type="cellIs" dxfId="69" priority="70" operator="lessThan">
+  <conditionalFormatting sqref="C92">
+    <cfRule type="cellIs" dxfId="69" priority="71" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C74">
-    <cfRule type="cellIs" dxfId="68" priority="69" operator="lessThan">
+  <conditionalFormatting sqref="C93 C95:C100">
+    <cfRule type="cellIs" dxfId="68" priority="70" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C75:C82">
-    <cfRule type="cellIs" dxfId="67" priority="68" operator="lessThan">
+  <conditionalFormatting sqref="C101">
+    <cfRule type="cellIs" dxfId="67" priority="69" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C83">
-    <cfRule type="cellIs" dxfId="66" priority="67" operator="lessThan">
+  <conditionalFormatting sqref="C102">
+    <cfRule type="cellIs" dxfId="66" priority="68" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C84 C87:C91">
-    <cfRule type="cellIs" dxfId="65" priority="66" operator="lessThan">
+  <conditionalFormatting sqref="C45:C46">
+    <cfRule type="cellIs" dxfId="65" priority="67" operator="lessThan">
+      <formula>0.012</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64:C65">
+    <cfRule type="cellIs" dxfId="64" priority="66" operator="lessThan">
+      <formula>0.012</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C85:C86">
+    <cfRule type="cellIs" dxfId="63" priority="65" operator="lessThan">
+      <formula>0.012</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C94">
+    <cfRule type="cellIs" dxfId="62" priority="64" operator="lessThan">
+      <formula>0.012</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E126:E133">
+    <cfRule type="cellIs" dxfId="61" priority="63" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E134">
+    <cfRule type="cellIs" dxfId="60" priority="62" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E135:E142">
+    <cfRule type="cellIs" dxfId="59" priority="61" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E143">
+    <cfRule type="cellIs" dxfId="58" priority="60" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E144:E149">
+    <cfRule type="cellIs" dxfId="57" priority="59" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E99:E106">
+    <cfRule type="cellIs" dxfId="56" priority="58" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E108">
+    <cfRule type="cellIs" dxfId="55" priority="57" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E109:E116">
+    <cfRule type="cellIs" dxfId="54" priority="56" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E117">
+    <cfRule type="cellIs" dxfId="53" priority="55" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E118:E125">
+    <cfRule type="cellIs" dxfId="52" priority="54" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52:E59">
+    <cfRule type="cellIs" dxfId="51" priority="53" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E60">
+    <cfRule type="cellIs" dxfId="50" priority="52" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E61:E68">
+    <cfRule type="cellIs" dxfId="49" priority="51" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69">
+    <cfRule type="cellIs" dxfId="48" priority="50" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E70:E77">
+    <cfRule type="cellIs" dxfId="47" priority="49" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E78">
+    <cfRule type="cellIs" dxfId="46" priority="48" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E79:E86">
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E87">
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E88:E95">
+    <cfRule type="cellIs" dxfId="43" priority="45" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E96">
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E97:E98">
+    <cfRule type="cellIs" dxfId="41" priority="43" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E11">
+    <cfRule type="cellIs" dxfId="40" priority="42" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="39" priority="41" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13:E20">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="cellIs" dxfId="37" priority="39" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22:E29">
+    <cfRule type="cellIs" dxfId="36" priority="38" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E33">
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35:E39">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41:E47">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C125:C132">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C92">
-    <cfRule type="cellIs" dxfId="64" priority="65" operator="lessThan">
+  <conditionalFormatting sqref="C133">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C93 C95:C100">
-    <cfRule type="cellIs" dxfId="63" priority="64" operator="lessThan">
+  <conditionalFormatting sqref="C137:C141">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C101">
-    <cfRule type="cellIs" dxfId="62" priority="63" operator="lessThan">
+  <conditionalFormatting sqref="C142">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C102">
-    <cfRule type="cellIs" dxfId="61" priority="62" operator="lessThan">
+  <conditionalFormatting sqref="C143 C145:C149">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="60" priority="61" operator="lessThan">
+  <conditionalFormatting sqref="C103:C105">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="lessThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C108 C110:C111">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="lessThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C112">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="lessThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C114:C117 C119:C120">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="lessThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C121">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="lessThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C122:C124">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="lessThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C109">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C64:C65">
-    <cfRule type="cellIs" dxfId="59" priority="60" operator="lessThan">
+  <conditionalFormatting sqref="C113">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C85:C86">
-    <cfRule type="cellIs" dxfId="58" priority="59" operator="lessThan">
+  <conditionalFormatting sqref="C118">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C94">
-    <cfRule type="cellIs" dxfId="57" priority="58" operator="lessThan">
+  <conditionalFormatting sqref="C134:C136">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E126:E133">
-    <cfRule type="cellIs" dxfId="56" priority="57" operator="lessThan">
+  <conditionalFormatting sqref="C144">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="lessThan">
+      <formula>0.012</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E150:E157">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E134">
-    <cfRule type="cellIs" dxfId="55" priority="56" operator="lessThan">
+  <conditionalFormatting sqref="E158">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E135:E142">
-    <cfRule type="cellIs" dxfId="54" priority="55" operator="lessThan">
+  <conditionalFormatting sqref="E159:E166">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E143">
-    <cfRule type="cellIs" dxfId="53" priority="54" operator="lessThan">
+  <conditionalFormatting sqref="E167">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E144:E149">
-    <cfRule type="cellIs" dxfId="52" priority="53" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E99:E106">
-    <cfRule type="cellIs" dxfId="51" priority="52" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E108">
-    <cfRule type="cellIs" dxfId="50" priority="51" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E109:E116">
-    <cfRule type="cellIs" dxfId="49" priority="50" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E117">
-    <cfRule type="cellIs" dxfId="48" priority="49" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E118:E125">
-    <cfRule type="cellIs" dxfId="47" priority="48" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52:E59">
-    <cfRule type="cellIs" dxfId="46" priority="47" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E60">
-    <cfRule type="cellIs" dxfId="45" priority="46" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E61:E68">
-    <cfRule type="cellIs" dxfId="44" priority="45" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
-    <cfRule type="cellIs" dxfId="43" priority="44" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E70:E77">
-    <cfRule type="cellIs" dxfId="42" priority="43" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E78">
-    <cfRule type="cellIs" dxfId="41" priority="42" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E79:E86">
-    <cfRule type="cellIs" dxfId="40" priority="41" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E87">
-    <cfRule type="cellIs" dxfId="39" priority="40" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E88:E95">
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E96">
-    <cfRule type="cellIs" dxfId="37" priority="38" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E97:E98">
-    <cfRule type="cellIs" dxfId="36" priority="37" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E11">
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="34" priority="35" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13:E20">
-    <cfRule type="cellIs" dxfId="33" priority="34" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="32" priority="33" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E29">
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="30" priority="31" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31:E33">
-    <cfRule type="cellIs" dxfId="29" priority="30" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35:E39">
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="27" priority="28" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41:E47">
-    <cfRule type="cellIs" dxfId="26" priority="27" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E50">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="lessThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C125:C132">
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="lessThan">
-      <formula>0.25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C133">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="lessThan">
-      <formula>0.25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C137:C141">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="lessThan">
-      <formula>0.25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C142">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="lessThan">
-      <formula>0.25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C143 C145:C149">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="lessThan">
-      <formula>0.25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C103:C105">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="lessThan">
-      <formula>0.25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C108 C110:C111">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="lessThan">
-      <formula>0.25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C112">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
-      <formula>0.25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C114:C117 C119:C120">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="lessThan">
-      <formula>0.25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C121">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="lessThan">
-      <formula>0.25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C122:C124">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
-      <formula>0.25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C109">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
-      <formula>0.012</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C113">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
-      <formula>0.012</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C118">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
-      <formula>0.012</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C134:C136">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
-      <formula>0.012</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C144">
+  <conditionalFormatting sqref="C106">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
       <formula>0.012</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E150:E157">
+  <conditionalFormatting sqref="E168:E174">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E158">
+  <conditionalFormatting sqref="E175:E188">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E159:E166">
+  <conditionalFormatting sqref="E189:E209">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E167">
+  <conditionalFormatting sqref="E211:E277">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E168">
+  <conditionalFormatting sqref="E278:E293">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C106">
+  <conditionalFormatting sqref="E295:E296">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
-      <formula>0.012</formula>
+      <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>